<commit_message>
Add of  the diagram title in cell J2 of excel sheet. Define the sheet name as to be Planning
</commit_message>
<xml_diff>
--- a/taches_et_jalons.xlsx
+++ b/taches_et_jalons.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Planning" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,6 +468,26 @@
           <t>End</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 7</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 8</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 9</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -492,6 +512,18 @@
       <c r="F2" s="2" t="n">
         <v>45542</v>
       </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Project title:</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>My Gantt diagram</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -516,6 +548,10 @@
       <c r="F3" s="2" t="n">
         <v>45541</v>
       </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -538,6 +574,10 @@
       <c r="F4" s="2" t="n">
         <v>45553</v>
       </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -562,6 +602,10 @@
       <c r="F5" s="2" t="n">
         <v>45555</v>
       </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -586,6 +630,10 @@
       <c r="F6" s="2" t="n">
         <v>45566</v>
       </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>